<commit_message>
Add keywords, update checklist
</commit_message>
<xml_diff>
--- a/Security_Code_Review_Helper.xlsx
+++ b/Security_Code_Review_Helper.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24102"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24110"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\KBCH8461\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A9D08491-834D-4DA8-B071-00F1037322F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="60" documentId="13_ncr:1_{F1123B4F-954A-4DE1-87D2-2033067BF9FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{270619D8-56CF-450F-9FAD-C804CA97FAC9}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="14505" firstSheet="3" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="14505" firstSheet="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Code Review Process" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="131">
   <si>
     <t>Check to perform</t>
   </si>
@@ -137,7 +137,7 @@
     <t>Hot spot checking</t>
   </si>
   <si>
-    <t>Using grep to target interesting keywords such as "password", "sql", etc.. Keyword list must be specific to the audited application</t>
+    <t>Using grep to target interesting keywords such as "password", "sql", etc.. Keyword list must be specific to the audited application. Megagrep + Graudit + Dumpsterdriver.</t>
   </si>
   <si>
     <t>Control flow sensitive</t>
@@ -421,10 +421,14 @@
     <t>A checklist is never exhaustive because application-specific functionalities comes with their own flaws. There is a high chance that business-logic flaws appear in the code.</t>
   </si>
   <si>
-    <t>XXE</t>
-  </si>
-  <si>
-    <t>CSRF</t>
+    <t>Web-specific</t>
+  </si>
+  <si>
+    <t>• CSRF
+• XEE
+• CORS
+• WebSockets
+• WebMessages</t>
   </si>
   <si>
     <t>Centralized checks</t>
@@ -1096,36 +1100,6 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1138,6 +1112,27 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1145,13 +1140,22 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="59">
+  <dxfs count="56">
     <dxf>
       <font>
         <color theme="7"/>
@@ -1229,36 +1233,6 @@
       <fill>
         <patternFill patternType="solid">
           <bgColor rgb="FFFF9393"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="7"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="4"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2059,8 +2033,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D58"/>
   <sheetViews>
-    <sheetView topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -2087,12 +2061,12 @@
       </c>
     </row>
     <row r="2" spans="1:4" ht="22.5" customHeight="1">
-      <c r="A2" s="34" t="s">
+      <c r="A2" s="42" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="35"/>
-      <c r="C2" s="35"/>
-      <c r="D2" s="35"/>
+      <c r="B2" s="43"/>
+      <c r="C2" s="43"/>
+      <c r="D2" s="43"/>
     </row>
     <row r="3" spans="1:4" ht="42" customHeight="1">
       <c r="A3" s="24" t="s">
@@ -2151,12 +2125,12 @@
       <c r="D7" s="27"/>
     </row>
     <row r="8" spans="1:4" ht="22.5" customHeight="1">
-      <c r="A8" s="34" t="s">
+      <c r="A8" s="42" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="35"/>
-      <c r="C8" s="35"/>
-      <c r="D8" s="35"/>
+      <c r="B8" s="43"/>
+      <c r="C8" s="43"/>
+      <c r="D8" s="43"/>
     </row>
     <row r="9" spans="1:4" ht="71.25" customHeight="1">
       <c r="A9" s="24" t="s">
@@ -2193,12 +2167,12 @@
       <c r="D11" s="27"/>
     </row>
     <row r="12" spans="1:4" ht="24.75" customHeight="1">
-      <c r="A12" s="34" t="s">
+      <c r="A12" s="42" t="s">
         <v>20</v>
       </c>
-      <c r="B12" s="35"/>
-      <c r="C12" s="35"/>
-      <c r="D12" s="35"/>
+      <c r="B12" s="43"/>
+      <c r="C12" s="43"/>
+      <c r="D12" s="43"/>
     </row>
     <row r="13" spans="1:4" ht="92.25" customHeight="1">
       <c r="A13" s="24" t="s">
@@ -2237,12 +2211,12 @@
       <c r="D15" s="27"/>
     </row>
     <row r="16" spans="1:4" ht="41.25" customHeight="1">
-      <c r="A16" s="34" t="s">
+      <c r="A16" s="42" t="s">
         <v>27</v>
       </c>
-      <c r="B16" s="35"/>
-      <c r="C16" s="35"/>
-      <c r="D16" s="35"/>
+      <c r="B16" s="43"/>
+      <c r="C16" s="43"/>
+      <c r="D16" s="43"/>
     </row>
     <row r="17" spans="1:4" ht="25.5">
       <c r="A17" s="24" t="s">
@@ -2317,12 +2291,12 @@
       <c r="D22" s="27"/>
     </row>
     <row r="23" spans="1:4" ht="21.75" customHeight="1">
-      <c r="A23" s="34" t="s">
+      <c r="A23" s="42" t="s">
         <v>40</v>
       </c>
-      <c r="B23" s="35"/>
-      <c r="C23" s="35"/>
-      <c r="D23" s="35"/>
+      <c r="B23" s="43"/>
+      <c r="C23" s="43"/>
+      <c r="D23" s="43"/>
     </row>
     <row r="24" spans="1:4" ht="31.5" customHeight="1">
       <c r="A24" s="24" t="s">
@@ -2548,107 +2522,107 @@
     <mergeCell ref="A23:D23"/>
   </mergeCells>
   <conditionalFormatting sqref="C3">
-    <cfRule type="cellIs" dxfId="58" priority="22" operator="equal">
+    <cfRule type="cellIs" dxfId="55" priority="22" operator="equal">
       <formula>"CHECKED"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C3">
-    <cfRule type="cellIs" dxfId="57" priority="21" operator="equal">
+    <cfRule type="cellIs" dxfId="54" priority="21" operator="equal">
       <formula>"TODO"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C3">
-    <cfRule type="cellIs" dxfId="56" priority="20" operator="equal">
+    <cfRule type="cellIs" dxfId="53" priority="20" operator="equal">
       <formula>"WIP"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C4:C7">
-    <cfRule type="cellIs" dxfId="55" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="52" priority="18" operator="equal">
       <formula>"CHECKED"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C4:C7">
-    <cfRule type="cellIs" dxfId="54" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="51" priority="17" operator="equal">
       <formula>"TODO"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C4:C7">
-    <cfRule type="cellIs" dxfId="53" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="50" priority="16" operator="equal">
       <formula>"WIP"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C9:C11">
-    <cfRule type="cellIs" dxfId="52" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="49" priority="15" operator="equal">
       <formula>"CHECKED"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C9:C11">
-    <cfRule type="cellIs" dxfId="51" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="48" priority="14" operator="equal">
       <formula>"TODO"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C9:C11">
-    <cfRule type="cellIs" dxfId="50" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="47" priority="13" operator="equal">
       <formula>"WIP"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C17:C22">
-    <cfRule type="cellIs" dxfId="49" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="46" priority="12" operator="equal">
       <formula>"CHECKED"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C17:C22">
-    <cfRule type="cellIs" dxfId="48" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="45" priority="11" operator="equal">
       <formula>"TODO"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C17:C22">
-    <cfRule type="cellIs" dxfId="47" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="44" priority="10" operator="equal">
       <formula>"WIP"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C24:C30">
-    <cfRule type="cellIs" dxfId="46" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="43" priority="9" operator="equal">
       <formula>"CHECKED"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C24:C30">
-    <cfRule type="cellIs" dxfId="45" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="42" priority="8" operator="equal">
       <formula>"TODO"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C24:C30">
-    <cfRule type="cellIs" dxfId="44" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="41" priority="7" operator="equal">
       <formula>"WIP"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C31">
-    <cfRule type="cellIs" dxfId="43" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="40" priority="6" operator="equal">
       <formula>"CHECKED"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C31">
-    <cfRule type="cellIs" dxfId="42" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="39" priority="5" operator="equal">
       <formula>"TODO"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C31">
-    <cfRule type="cellIs" dxfId="41" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="38" priority="4" operator="equal">
       <formula>"WIP"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C13:C15">
-    <cfRule type="cellIs" dxfId="40" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="37" priority="3" operator="equal">
       <formula>"CHECKED"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C13:C15">
-    <cfRule type="cellIs" dxfId="39" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="36" priority="2" operator="equal">
       <formula>"TODO"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C13:C15">
-    <cfRule type="cellIs" dxfId="38" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="35" priority="1" operator="equal">
       <formula>"WIP"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2663,10 +2637,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B50ED78-5F6F-4459-8250-1BBE69BF86C5}">
-  <dimension ref="A1:D47"/>
+  <dimension ref="A1:D46"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="B43" sqref="B43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -2693,12 +2667,12 @@
       </c>
     </row>
     <row r="2" spans="1:4" ht="25.5" customHeight="1">
-      <c r="A2" s="37" t="s">
+      <c r="A2" s="45" t="s">
         <v>41</v>
       </c>
-      <c r="B2" s="37"/>
-      <c r="C2" s="37"/>
-      <c r="D2" s="37"/>
+      <c r="B2" s="45"/>
+      <c r="C2" s="45"/>
+      <c r="D2" s="45"/>
     </row>
     <row r="3" spans="1:4" ht="188.25" customHeight="1">
       <c r="A3" s="17" t="s">
@@ -2749,12 +2723,12 @@
       <c r="D6" s="18"/>
     </row>
     <row r="7" spans="1:4" ht="22.5" customHeight="1">
-      <c r="A7" s="38" t="s">
+      <c r="A7" s="46" t="s">
         <v>42</v>
       </c>
-      <c r="B7" s="39"/>
-      <c r="C7" s="39"/>
-      <c r="D7" s="40"/>
+      <c r="B7" s="47"/>
+      <c r="C7" s="47"/>
+      <c r="D7" s="48"/>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" s="17" t="s">
@@ -2825,12 +2799,12 @@
       <c r="D13" s="18"/>
     </row>
     <row r="14" spans="1:4" ht="26.25" customHeight="1">
-      <c r="A14" s="38" t="s">
+      <c r="A14" s="46" t="s">
         <v>43</v>
       </c>
-      <c r="B14" s="39"/>
-      <c r="C14" s="39"/>
-      <c r="D14" s="40"/>
+      <c r="B14" s="47"/>
+      <c r="C14" s="47"/>
+      <c r="D14" s="48"/>
     </row>
     <row r="15" spans="1:4" ht="38.25" customHeight="1">
       <c r="A15" s="17" t="s">
@@ -2913,12 +2887,12 @@
       <c r="D21" s="18"/>
     </row>
     <row r="22" spans="1:4" ht="21" customHeight="1">
-      <c r="A22" s="38" t="s">
+      <c r="A22" s="46" t="s">
         <v>44</v>
       </c>
-      <c r="B22" s="39"/>
-      <c r="C22" s="39"/>
-      <c r="D22" s="40"/>
+      <c r="B22" s="47"/>
+      <c r="C22" s="47"/>
+      <c r="D22" s="48"/>
     </row>
     <row r="23" spans="1:4" ht="97.5" customHeight="1">
       <c r="A23" s="17" t="s">
@@ -2945,12 +2919,12 @@
       <c r="D24" s="18"/>
     </row>
     <row r="25" spans="1:4" ht="24" customHeight="1">
-      <c r="A25" s="38" t="s">
+      <c r="A25" s="46" t="s">
         <v>45</v>
       </c>
-      <c r="B25" s="39"/>
-      <c r="C25" s="39"/>
-      <c r="D25" s="40"/>
+      <c r="B25" s="47"/>
+      <c r="C25" s="47"/>
+      <c r="D25" s="48"/>
     </row>
     <row r="26" spans="1:4" ht="81" customHeight="1">
       <c r="A26" s="17" t="s">
@@ -2989,12 +2963,12 @@
       <c r="D28" s="18"/>
     </row>
     <row r="29" spans="1:4" ht="23.25" customHeight="1">
-      <c r="A29" s="36" t="s">
+      <c r="A29" s="44" t="s">
         <v>46</v>
       </c>
-      <c r="B29" s="36"/>
-      <c r="C29" s="36"/>
-      <c r="D29" s="36"/>
+      <c r="B29" s="44"/>
+      <c r="C29" s="44"/>
+      <c r="D29" s="44"/>
     </row>
     <row r="30" spans="1:4" ht="84" customHeight="1">
       <c r="A30" s="17" t="s">
@@ -3033,12 +3007,12 @@
       <c r="D32" s="18"/>
     </row>
     <row r="33" spans="1:4" ht="20.25" customHeight="1">
-      <c r="A33" s="36" t="s">
+      <c r="A33" s="44" t="s">
         <v>47</v>
       </c>
-      <c r="B33" s="36"/>
-      <c r="C33" s="36"/>
-      <c r="D33" s="36"/>
+      <c r="B33" s="44"/>
+      <c r="C33" s="44"/>
+      <c r="D33" s="44"/>
     </row>
     <row r="34" spans="1:4" ht="79.5" customHeight="1">
       <c r="A34" s="17" t="s">
@@ -3077,12 +3051,12 @@
       <c r="D36" s="18"/>
     </row>
     <row r="37" spans="1:4" ht="22.5" customHeight="1">
-      <c r="A37" s="36" t="s">
+      <c r="A37" s="44" t="s">
         <v>48</v>
       </c>
-      <c r="B37" s="36"/>
-      <c r="C37" s="36"/>
-      <c r="D37" s="36"/>
+      <c r="B37" s="44"/>
+      <c r="C37" s="44"/>
+      <c r="D37" s="44"/>
     </row>
     <row r="38" spans="1:4" ht="45">
       <c r="A38" s="17" t="s">
@@ -3132,71 +3106,61 @@
       </c>
       <c r="D41" s="18"/>
     </row>
-    <row r="42" spans="1:4">
+    <row r="42" spans="1:4" ht="111.75" customHeight="1">
       <c r="A42" s="17" t="s">
         <v>108</v>
       </c>
-      <c r="B42" s="18"/>
-      <c r="C42" s="19" t="s">
-        <v>7</v>
-      </c>
+      <c r="B42" s="18" t="s">
+        <v>109</v>
+      </c>
+      <c r="C42" s="19"/>
       <c r="D42" s="18"/>
     </row>
-    <row r="43" spans="1:4">
+    <row r="43" spans="1:4" ht="30">
       <c r="A43" s="17" t="s">
-        <v>109</v>
-      </c>
-      <c r="B43" s="18"/>
+        <v>110</v>
+      </c>
+      <c r="B43" s="18" t="s">
+        <v>111</v>
+      </c>
       <c r="C43" s="19" t="s">
         <v>7</v>
       </c>
       <c r="D43" s="18"/>
     </row>
-    <row r="44" spans="1:4" ht="30">
-      <c r="A44" s="17" t="s">
-        <v>110</v>
-      </c>
-      <c r="B44" s="18" t="s">
-        <v>111</v>
-      </c>
+    <row r="44" spans="1:4" ht="45" customHeight="1">
+      <c r="A44" s="20" t="s">
+        <v>112</v>
+      </c>
+      <c r="B44" s="18"/>
       <c r="C44" s="19" t="s">
         <v>7</v>
       </c>
       <c r="D44" s="18"/>
     </row>
     <row r="45" spans="1:4" ht="45" customHeight="1">
-      <c r="A45" s="20" t="s">
-        <v>112</v>
-      </c>
-      <c r="B45" s="18"/>
+      <c r="A45" s="21" t="s">
+        <v>113</v>
+      </c>
+      <c r="B45" s="22" t="s">
+        <v>114</v>
+      </c>
       <c r="C45" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="D45" s="18"/>
-    </row>
-    <row r="46" spans="1:4" ht="45" customHeight="1">
-      <c r="A46" s="21" t="s">
-        <v>113</v>
+      <c r="D45" s="22"/>
+    </row>
+    <row r="46" spans="1:4" ht="86.25" customHeight="1">
+      <c r="A46" s="23" t="s">
+        <v>115</v>
       </c>
       <c r="B46" s="22" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="C46" s="19" t="s">
         <v>7</v>
       </c>
       <c r="D46" s="22"/>
-    </row>
-    <row r="47" spans="1:4" ht="86.25" customHeight="1">
-      <c r="A47" s="23" t="s">
-        <v>115</v>
-      </c>
-      <c r="B47" s="22" t="s">
-        <v>116</v>
-      </c>
-      <c r="C47" s="19" t="s">
-        <v>7</v>
-      </c>
-      <c r="D47" s="22"/>
     </row>
   </sheetData>
   <mergeCells count="8">
@@ -3209,123 +3173,108 @@
     <mergeCell ref="A22:D22"/>
     <mergeCell ref="A25:D25"/>
   </mergeCells>
-  <conditionalFormatting sqref="C3:C6">
-    <cfRule type="cellIs" dxfId="37" priority="27" operator="equal">
+  <conditionalFormatting sqref="C3:C6 C38:C46">
+    <cfRule type="cellIs" dxfId="34" priority="27" operator="equal">
       <formula>"CHECKED"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C3:C6">
-    <cfRule type="cellIs" dxfId="36" priority="26" operator="equal">
+  <conditionalFormatting sqref="C3:C6 C38:C46">
+    <cfRule type="cellIs" dxfId="33" priority="26" operator="equal">
       <formula>"TODO"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C3:C6">
-    <cfRule type="cellIs" dxfId="35" priority="25" operator="equal">
+  <conditionalFormatting sqref="C3:C6 C38:C46">
+    <cfRule type="cellIs" dxfId="32" priority="25" operator="equal">
       <formula>"WIP"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C16:C21">
-    <cfRule type="cellIs" dxfId="34" priority="24" operator="equal">
+    <cfRule type="cellIs" dxfId="31" priority="24" operator="equal">
       <formula>"CHECKED"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C16:C21">
-    <cfRule type="cellIs" dxfId="33" priority="23" operator="equal">
+    <cfRule type="cellIs" dxfId="30" priority="23" operator="equal">
       <formula>"TODO"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C16:C21">
-    <cfRule type="cellIs" dxfId="32" priority="22" operator="equal">
+    <cfRule type="cellIs" dxfId="29" priority="22" operator="equal">
       <formula>"WIP"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C15">
-    <cfRule type="cellIs" dxfId="31" priority="21" operator="equal">
+    <cfRule type="cellIs" dxfId="28" priority="21" operator="equal">
       <formula>"CHECKED"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C15">
-    <cfRule type="cellIs" dxfId="30" priority="20" operator="equal">
+    <cfRule type="cellIs" dxfId="27" priority="20" operator="equal">
       <formula>"TODO"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C15">
-    <cfRule type="cellIs" dxfId="29" priority="19" operator="equal">
+    <cfRule type="cellIs" dxfId="26" priority="19" operator="equal">
       <formula>"WIP"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C8:C13">
-    <cfRule type="cellIs" dxfId="28" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="25" priority="18" operator="equal">
       <formula>"CHECKED"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C8:C13">
-    <cfRule type="cellIs" dxfId="27" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="17" operator="equal">
       <formula>"TODO"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C8:C13">
-    <cfRule type="cellIs" dxfId="26" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="16" operator="equal">
       <formula>"WIP"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C26:C28">
-    <cfRule type="cellIs" dxfId="25" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="15" operator="equal">
       <formula>"CHECKED"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C26:C28">
-    <cfRule type="cellIs" dxfId="24" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="14" operator="equal">
       <formula>"TODO"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C26:C28">
-    <cfRule type="cellIs" dxfId="23" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="13" operator="equal">
       <formula>"WIP"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C30:C32">
-    <cfRule type="cellIs" dxfId="22" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="12" operator="equal">
       <formula>"CHECKED"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C30:C32">
-    <cfRule type="cellIs" dxfId="21" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="11" operator="equal">
       <formula>"TODO"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C30:C32">
-    <cfRule type="cellIs" dxfId="20" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="10" operator="equal">
       <formula>"WIP"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C34:C36">
-    <cfRule type="cellIs" dxfId="19" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="9" operator="equal">
       <formula>"CHECKED"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C34:C36">
-    <cfRule type="cellIs" dxfId="18" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="8" operator="equal">
       <formula>"TODO"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C34:C36">
-    <cfRule type="cellIs" dxfId="17" priority="7" operator="equal">
-      <formula>"WIP"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C38:C47">
-    <cfRule type="cellIs" dxfId="16" priority="6" operator="equal">
-      <formula>"CHECKED"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C38:C47">
-    <cfRule type="cellIs" dxfId="15" priority="5" operator="equal">
-      <formula>"TODO"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C38:C47">
-    <cfRule type="cellIs" dxfId="14" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="7" operator="equal">
       <formula>"WIP"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3345,7 +3294,7 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="C3:C6 C15:C21 C8:C13 C26:C28 C30:C32 C34:C36 C38:C47 C23:C24" xr:uid="{4E754388-5615-4552-A879-81E58A3BC7DD}">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="C3:C6 C15:C21 C8:C13 C26:C28 C30:C32 C34:C36 C23:C24 C38:C46" xr:uid="{4E754388-5615-4552-A879-81E58A3BC7DD}">
       <formula1>"TODO, WIP, CHECKED"</formula1>
     </dataValidation>
   </dataValidations>
@@ -3425,7 +3374,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D35D9A02-EFE7-4C87-A78F-4132C5A58C57}">
   <dimension ref="A1:J7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
@@ -3443,35 +3392,35 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="15.75">
-      <c r="A1" s="52" t="s">
+      <c r="A1" s="49" t="s">
         <v>119</v>
       </c>
-      <c r="B1" s="53"/>
-      <c r="C1" s="53"/>
-      <c r="D1" s="53"/>
-      <c r="E1" s="54"/>
-      <c r="F1" s="43" t="s">
+      <c r="B1" s="50"/>
+      <c r="C1" s="50"/>
+      <c r="D1" s="50"/>
+      <c r="E1" s="51"/>
+      <c r="F1" s="52" t="s">
         <v>120</v>
       </c>
-      <c r="G1" s="43"/>
-      <c r="H1" s="43"/>
-      <c r="I1" s="41"/>
-      <c r="J1" s="42"/>
+      <c r="G1" s="52"/>
+      <c r="H1" s="52"/>
+      <c r="I1" s="53"/>
+      <c r="J1" s="54"/>
     </row>
     <row r="2" spans="1:10">
-      <c r="A2" s="44" t="s">
+      <c r="A2" s="34" t="s">
         <v>121</v>
       </c>
-      <c r="B2" s="45" t="s">
+      <c r="B2" s="35" t="s">
         <v>122</v>
       </c>
-      <c r="C2" s="45" t="s">
+      <c r="C2" s="35" t="s">
         <v>123</v>
       </c>
-      <c r="D2" s="45" t="s">
+      <c r="D2" s="35" t="s">
         <v>124</v>
       </c>
-      <c r="E2" s="46" t="s">
+      <c r="E2" s="36" t="s">
         <v>125</v>
       </c>
       <c r="F2" s="10" t="s">
@@ -3491,11 +3440,11 @@
       </c>
     </row>
     <row r="3" spans="1:10">
-      <c r="A3" s="47"/>
+      <c r="A3" s="37"/>
       <c r="B3" s="11"/>
       <c r="C3" s="11"/>
       <c r="D3" s="11"/>
-      <c r="E3" s="48" t="s">
+      <c r="E3" s="38" t="s">
         <v>7</v>
       </c>
       <c r="G3" s="32"/>
@@ -3504,11 +3453,11 @@
       <c r="J3" s="13"/>
     </row>
     <row r="4" spans="1:10">
-      <c r="A4" s="47"/>
+      <c r="A4" s="37"/>
       <c r="B4" s="11"/>
       <c r="C4" s="11"/>
       <c r="D4" s="11"/>
-      <c r="E4" s="48" t="s">
+      <c r="E4" s="38" t="s">
         <v>7</v>
       </c>
       <c r="F4" s="32"/>
@@ -3518,11 +3467,11 @@
       <c r="J4" s="13"/>
     </row>
     <row r="5" spans="1:10">
-      <c r="A5" s="47"/>
+      <c r="A5" s="37"/>
       <c r="B5" s="11"/>
       <c r="C5" s="11"/>
       <c r="D5" s="11"/>
-      <c r="E5" s="48" t="s">
+      <c r="E5" s="38" t="s">
         <v>7</v>
       </c>
       <c r="F5" s="32"/>
@@ -3532,11 +3481,11 @@
       <c r="J5" s="13"/>
     </row>
     <row r="6" spans="1:10">
-      <c r="A6" s="47"/>
+      <c r="A6" s="37"/>
       <c r="B6" s="11"/>
       <c r="C6" s="11"/>
       <c r="D6" s="11"/>
-      <c r="E6" s="48" t="s">
+      <c r="E6" s="38" t="s">
         <v>7</v>
       </c>
       <c r="F6" s="32"/>
@@ -3546,11 +3495,11 @@
       <c r="J6" s="13"/>
     </row>
     <row r="7" spans="1:10">
-      <c r="A7" s="49"/>
-      <c r="B7" s="50"/>
-      <c r="C7" s="50"/>
-      <c r="D7" s="50"/>
-      <c r="E7" s="51" t="s">
+      <c r="A7" s="39"/>
+      <c r="B7" s="40"/>
+      <c r="C7" s="40"/>
+      <c r="D7" s="40"/>
+      <c r="E7" s="41" t="s">
         <v>7</v>
       </c>
       <c r="F7" s="33"/>

</xml_diff>